<commit_message>
Final version of dataset
</commit_message>
<xml_diff>
--- a/gen/cormat.xlsx
+++ b/gen/cormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c2a02be2a6fea48/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajthurston/Documents/GitHub/validation/gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{65662A43-0D3B-45D9-9B15-FEF95EFE1A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85EB8499-3032-491C-82D6-BBEABE8A3E31}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D4C48-5787-9B42-B2F3-F75982CC1EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{9EC584D0-7A16-425A-8CA4-CF8095FF7F2E}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{9EC584D0-7A16-425A-8CA4-CF8095FF7F2E}"/>
   </bookViews>
   <sheets>
     <sheet name="cor" sheetId="1" r:id="rId1"/>
@@ -189,10 +189,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,12 +491,12 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="A1:Y26"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -606,7 +602,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -637,7 +633,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -670,7 +666,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -705,7 +701,7 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -742,7 +738,7 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -781,7 +777,7 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0</v>
       </c>
@@ -822,7 +818,7 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
@@ -865,7 +861,7 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>0.15</v>
       </c>
@@ -910,7 +906,7 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0.05</v>
       </c>
@@ -957,12 +953,12 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>-0.5</v>
+        <v>0.2</v>
       </c>
       <c r="B12" s="3">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="C12" s="3">
         <v>0.2</v>
@@ -1006,9 +1002,9 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>-0.5</v>
+        <v>0.2</v>
       </c>
       <c r="B13" s="3">
         <v>-0.2</v>
@@ -1057,12 +1053,12 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>-0.5</v>
+        <v>0.2</v>
       </c>
       <c r="B14" s="3">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="C14" s="3">
         <v>0.2</v>
@@ -1110,24 +1106,24 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="B15" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C15" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D15" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E15" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F15" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G15" s="2">
         <v>-0.03</v>
@@ -1165,24 +1161,24 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="B16" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C16" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D16" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E16" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F16" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G16" s="2">
         <v>-0.1</v>
@@ -1222,24 +1218,24 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="B17" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C17" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D17" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E17" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F17" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G17" s="2">
         <v>-0.2</v>
@@ -1281,24 +1277,24 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="B18" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C18" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D18" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E18" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F18" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G18" s="2">
         <v>-0.3</v>
@@ -1342,24 +1338,24 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="B19" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C19" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D19" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E19" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -1383,16 +1379,16 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="N19" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="O19" s="2">
-        <v>0.26700000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="P19" s="2">
-        <v>0.24199999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="Q19" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="R19" s="2">
         <v>1</v>
@@ -1405,24 +1401,24 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="B20" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C20" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D20" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E20" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F20" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
@@ -1449,13 +1445,13 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="O20" s="2">
-        <v>0.24199999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="P20" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="Q20" s="2">
-        <v>0.26700000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="R20" s="2">
         <v>0.78</v>
@@ -1470,24 +1466,24 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="B21" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C21" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D21" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E21" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F21" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G21" s="2">
         <v>0.1</v>
@@ -1514,13 +1510,13 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="O21" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="P21" s="2">
-        <v>0.26700000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="Q21" s="2">
-        <v>0.24199999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="R21" s="2">
         <v>0.92</v>
@@ -1537,24 +1533,24 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="B22" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C22" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D22" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E22" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F22" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G22" s="2">
         <v>-0.1</v>
@@ -1581,13 +1577,13 @@
         <v>0.29299999999999998</v>
       </c>
       <c r="O22" s="2">
-        <v>0.26700000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="P22" s="2">
-        <v>0.24199999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="Q22" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="R22" s="2">
         <v>0.84</v>
@@ -1606,24 +1602,24 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="B23" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C23" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E23" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F23" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G23" s="2">
         <v>0.2</v>
@@ -1677,24 +1673,24 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="B24" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C24" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D24" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E24" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F24" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G24" s="2">
         <v>0.3</v>
@@ -1750,24 +1746,24 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="B25" s="4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C25" s="4">
-        <v>-0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D25" s="4">
-        <v>-0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E25" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="F25" s="4">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="G25" s="2">
         <v>0.35</v>
@@ -1825,7 +1821,7 @@
       </c>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -1881,13 +1877,13 @@
         <v>0.4</v>
       </c>
       <c r="S26" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="T26" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="U26" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="V26" s="3">
         <v>0.4</v>
@@ -1902,7 +1898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="E27" s="2"/>
     </row>
   </sheetData>
@@ -1922,9 +1918,9 @@
       <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +1997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2091,9 +2087,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.7</v>
       </c>
@@ -2247,7 +2243,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -2263,9 +2259,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2273,7 +2269,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2281,7 +2277,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2289,7 +2285,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2297,7 +2293,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2305,7 +2301,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2313,7 +2309,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2321,7 +2317,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2329,7 +2325,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2337,7 +2333,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2345,7 +2341,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2353,7 +2349,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2361,7 +2357,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2369,7 +2365,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2377,7 +2373,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2385,7 +2381,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2393,7 +2389,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2401,7 +2397,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2409,7 +2405,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2417,7 +2413,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -2425,7 +2421,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2433,7 +2429,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2441,7 +2437,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2449,7 +2445,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -2457,7 +2453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>

</xml_diff>